<commit_message>
Added % to info
Did manually in excel
</commit_message>
<xml_diff>
--- a/Compiled outputs Feb 2025.xlsx
+++ b/Compiled outputs Feb 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\md1rwe\Documents\Data extractions from I-CAH\Feb 2025\I-CAH_data_Feb_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67CEE7-12BD-4C5A-BFCA-3604045FCA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8E5D09-BF99-448E-8E70-4C8A7A50B616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="5595" windowWidth="31605" windowHeight="12375" activeTab="1" xr2:uid="{0C64CAD2-99F8-4483-9AFB-7830603B63CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3" xr2:uid="{0C64CAD2-99F8-4483-9AFB-7830603B63CF}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1973" uniqueCount="295">
   <si>
     <t>Sex.at.birth</t>
   </si>
@@ -954,11 +954,23 @@
   <si>
     <t>number of centres</t>
   </si>
+  <si>
+    <t>total records</t>
+  </si>
+  <si>
+    <t>percentages</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1091,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1101,6 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,7 +1123,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,7 +1468,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>278</v>
       </c>
     </row>
@@ -1467,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A940C76-8F58-433A-A718-D5E484B5CF3F}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240E7E16-AC56-4C11-904F-02087C4BEB65}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,39 +1812,54 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>245</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="13">
+        <f>B2/SUM($B$2:$B$4) * 100</f>
+        <v>62.340966921119588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="13">
+        <f>B3/SUM($B$2:$B$4) * 100</f>
+        <v>37.404580152671755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="13">
+        <f t="shared" ref="C3:C4" si="0">B4/SUM($B$2:$B$4) * 100</f>
+        <v>0.2544529262086514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>276</v>
       </c>
@@ -1848,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A111D79-B485-43F1-84B3-3B22599F6023}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,6 +1893,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1872,6 +1904,10 @@
       <c r="B2">
         <v>70</v>
       </c>
+      <c r="C2" s="13">
+        <f>B2/SUM($B$2:$B$8) * 100</f>
+        <v>17.8117048346056</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1880,6 +1916,10 @@
       <c r="B3">
         <v>112</v>
       </c>
+      <c r="C3" s="13">
+        <f t="shared" ref="C3:C8" si="0">B3/SUM($B$2:$B$8) * 100</f>
+        <v>28.498727735368956</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1888,6 +1928,10 @@
       <c r="B4">
         <v>95</v>
       </c>
+      <c r="C4" s="13">
+        <f t="shared" si="0"/>
+        <v>24.173027989821882</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1896,6 +1940,10 @@
       <c r="B5">
         <v>62</v>
       </c>
+      <c r="C5" s="13">
+        <f t="shared" si="0"/>
+        <v>15.776081424936386</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1904,6 +1952,10 @@
       <c r="B6">
         <v>35</v>
       </c>
+      <c r="C6" s="13">
+        <f t="shared" si="0"/>
+        <v>8.9058524173027998</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1912,6 +1964,10 @@
       <c r="B7">
         <v>14</v>
       </c>
+      <c r="C7" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5623409669211195</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1919,6 +1975,10 @@
       </c>
       <c r="B8">
         <v>5</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="0"/>
+        <v>1.2722646310432568</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,39 +2019,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5097C6-8B27-4856-BBA5-3F7AAE1DEDDD}">
-  <dimension ref="B2:J4"/>
+  <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="9" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2020,7 +2082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -2048,6 +2110,67 @@
       <c r="J4" s="6">
         <v>2</v>
       </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="14">
+        <f>B4/SUM($B$4:$E$4) * 100</f>
+        <v>1.5873015873015872</v>
+      </c>
+      <c r="C6" s="14">
+        <f t="shared" ref="C6:F6" si="0">C4/SUM($B$4:$E$4) * 100</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F6" s="14">
+        <f>F4/SUM($F$4:$J$4) * 100</f>
+        <v>2.7027027027027026</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" ref="G6:J6" si="1">G4/SUM($F$4:$J$4) * 100</f>
+        <v>36.293436293436294</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="1"/>
+        <v>5.019305019305019</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="1"/>
+        <v>55.212355212355213</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.77220077220077221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8">
+        <f>SUM(B4:E4)</f>
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G8">
+        <f>SUM(F4:J4)</f>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2086,28 +2209,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11562,7 +11685,7 @@
   <dimension ref="B1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11572,22 +11695,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="I1" s="9" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">

</xml_diff>